<commit_message>
fix permission access in gl_receivable_report and template 11/10/2018
</commit_message>
<xml_diff>
--- a/pabi_account_report/xlsx_template/xlsx_report_gl_receivable.xlsx
+++ b/pabi_account_report/xlsx_template/xlsx_report_gl_receivable.xlsx
@@ -215,10 +215,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="MM"/>
-    <numFmt numFmtId="166" formatCode="DD/MM/YYYY"/>
+    <numFmt numFmtId="165" formatCode="DD/MM/YYYY"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -313,7 +312,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -329,7 +328,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -345,7 +344,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -437,7 +436,7 @@
   <dimension ref="A2:BB10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
+      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I:I"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
add prefix document for use common report 17/07/2018
</commit_message>
<xml_diff>
--- a/pabi_account_report/xlsx_template/xlsx_report_gl_receivable.xlsx
+++ b/pabi_account_report/xlsx_template/xlsx_report_gl_receivable.xlsx
@@ -100,10 +100,10 @@
     <t xml:space="preserve">Header Description</t>
   </si>
   <si>
-    <t xml:space="preserve">Document Type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Document Journal</t>
+    <t xml:space="preserve">Doc Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Doc Journal</t>
   </si>
   <si>
     <t xml:space="preserve">Internal Number</t>
@@ -433,8 +433,8 @@
   </sheetPr>
   <dimension ref="A1:BB12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O13" activeCellId="0" sqref="O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>